<commit_message>
modifying data processing and IC
</commit_message>
<xml_diff>
--- a/NC_filling_estimation/initial_conditions.xlsx
+++ b/NC_filling_estimation/initial_conditions.xlsx
@@ -48,40 +48,40 @@
     <t>wall dT</t>
   </si>
   <si>
-    <t>NC-MFR-ABS-1_5</t>
-  </si>
-  <si>
-    <t>NC-MFR_HE-ABS-1_5</t>
-  </si>
-  <si>
-    <t>NC-MFR-ABS-2</t>
-  </si>
-  <si>
-    <t>NC-MFR_HE-ABS-2</t>
-  </si>
-  <si>
-    <t>NC-MFR-ABS-2_5</t>
-  </si>
-  <si>
-    <t>NC-MFR_HE-ABS-2_5</t>
-  </si>
-  <si>
-    <t>NC-MFR-ABS-3</t>
-  </si>
-  <si>
-    <t>NC-MFR_HE-ABS-3</t>
-  </si>
-  <si>
     <t>NC-MFR-ABS-4</t>
   </si>
   <si>
     <t>NC-MFR_HE-ABS-4</t>
   </si>
   <si>
-    <t>NC-MFR-PART-1_5</t>
-  </si>
-  <si>
-    <t>NC-MFR-PART-2_5</t>
+    <t>NC-MFR-ABS-1_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-2_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-3_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-4_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-5_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-6_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-7_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-8_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-9_4</t>
+  </si>
+  <si>
+    <t>NC-MFR-ABS-10_4</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J3"/>
+      <selection sqref="A1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,28 +462,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>0.1265958758335281</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2.11</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>120.28261502915524</v>
+        <v>143.61253299838279</v>
       </c>
       <c r="H2">
-        <v>100.28261502915524</v>
+        <v>123.61253299838279</v>
       </c>
       <c r="I2">
         <v>2</v>
@@ -494,28 +494,28 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>0.36831663771905754</v>
+        <v>0.20890589895780506</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2.35</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>120.1720066632181</v>
+        <v>141.77262336984768</v>
       </c>
       <c r="H3">
-        <v>100.1720066632181</v>
+        <v>121.77262336984768</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -526,28 +526,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>0.2508220137803423</v>
+        <v>0.39614414590889629</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>149.91361092817692</v>
+        <v>139.85299129047138</v>
       </c>
       <c r="H4">
-        <v>129.91361092817692</v>
+        <v>119.85299129047138</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -558,28 +558,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>0.2508220137803423</v>
+        <v>0.58525134154773539</v>
       </c>
       <c r="C5">
-        <v>0.2508220137803423</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>149.91361092817692</v>
+        <v>137.84534219941258</v>
       </c>
       <c r="H5">
-        <v>129.91361092817692</v>
+        <v>117.84534219941258</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -590,28 +590,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>0.48041828670814996</v>
+        <v>0.77639494589316116</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>147.90809697170238</v>
+        <v>135.73996041273483</v>
       </c>
       <c r="H6">
-        <v>127.90809697170238</v>
+        <v>115.73996041273483</v>
       </c>
       <c r="I6">
         <v>2</v>
@@ -622,28 +622,28 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>0.48041828670814996</v>
+        <v>0.96977146449668861</v>
       </c>
       <c r="C7">
-        <v>0.48041828670814996</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>147.90809697170238</v>
+        <v>133.52535794654545</v>
       </c>
       <c r="H7">
-        <v>127.90809697170238</v>
+        <v>113.52535794654545</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -654,28 +654,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>0.71236268503630196</v>
+        <v>1.1656126975459682</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>145.81109686110756</v>
+        <v>131.18780629572507</v>
       </c>
       <c r="H8">
-        <v>125.81109686110756</v>
+        <v>111.18780629572507</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -686,28 +686,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>0.71236268503630196</v>
+        <v>1.565862322646411</v>
       </c>
       <c r="C9">
-        <v>0.71236268503630196</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>145.81109686110756</v>
+        <v>126.07367775380408</v>
       </c>
       <c r="H9">
-        <v>125.81109686110756</v>
+        <v>106.07367775380408</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -718,28 +718,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B10">
-        <v>0.94686550962079596</v>
+        <v>1.9802133138045936</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>143.61253299838279</v>
+        <v>120.21154593648862</v>
       </c>
       <c r="H10">
-        <v>123.61253299838279</v>
+        <v>100.21154593648862</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -750,28 +750,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B11">
-        <v>0.94686550962079596</v>
+        <v>2.6398920519333142</v>
       </c>
       <c r="C11">
-        <v>0.94686550962079596</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.2</v>
+        <v>0.65</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>143.61253299838279</v>
+        <v>109.29210588198293</v>
       </c>
       <c r="H11">
-        <v>123.61253299838279</v>
+        <v>89.292105881982934</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1.4245782176988584</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1.4245782176988584</v>

</xml_diff>